<commit_message>
Update schedule file: Y2_B2425_Blood_&_lymphatics_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y2_B2425_Blood_&_lymphatics_schedule.xlsx
+++ b/modules_schedules/Y2_B2425_Blood_&_lymphatics_schedule.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,12 +522,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>21/09/2025</t>
+          <t>22/09/2025</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D3" s="5" t="inlineStr">
@@ -569,12 +569,12 @@
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>22/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F3" s="7" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -601,12 +601,12 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>22/09/2025</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>09:00:00</t>
         </is>
       </c>
     </row>
@@ -628,17 +628,17 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
-          <t>22/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
-          <t>09:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
     </row>
@@ -650,27 +650,27 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>22/09/2025</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>11:00:00</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
@@ -697,12 +697,12 @@
       </c>
       <c r="E7" s="6" t="inlineStr">
         <is>
-          <t>22/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
-          <t>11:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -729,12 +729,12 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>22/09/2025</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E9" s="6" t="inlineStr">
         <is>
-          <t>22/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F9" s="7" t="inlineStr">
@@ -778,17 +778,17 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E11" s="6" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
     </row>
@@ -842,27 +842,27 @@
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C4</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>23/09/2025</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
@@ -889,12 +889,12 @@
       </c>
       <c r="E13" s="6" t="inlineStr">
         <is>
-          <t>23/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F13" s="7" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -921,12 +921,12 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>25/09/2025</t>
+          <t>23/09/2025</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
     </row>
@@ -948,47 +948,15 @@
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E15" s="6" t="inlineStr">
         <is>
-          <t>23/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="F15" s="7" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>C4</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>physiology</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>25/09/2025</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>

</xml_diff>